<commit_message>
Add script to identify key genes in each disease gene list
</commit_message>
<xml_diff>
--- a/results/humanPVATsn/pathfindR/full/Sonia_network/full_diff_sonia.xlsx
+++ b/results/humanPVATsn/pathfindR/full/Sonia_network/full_diff_sonia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\LN2PEPF0000C39F\EXCELCNV\c97d3396-8130-47ce-a108-7fe796139769\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahbazin/Desktop/Cambridge/Academics/Han_Lab/MPhil/mphil-project/results/humanPVATsn/pathfindR/full/Sonia_network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{7CB3B77A-AABF-4C59-9EA2-2CFE73789634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0AE07AE-B3B2-4491-994E-DEBC6B0F2E42}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6519817A-EBCD-0F43-ABE4-1F65B8FBB881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{55FB20EB-352A-4374-8085-867F7A25DBE2}"/>
+    <workbookView xWindow="-5100" yWindow="-21100" windowWidth="28720" windowHeight="19100" xr2:uid="{55FB20EB-352A-4374-8085-867F7A25DBE2}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -3117,7 +3117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3664,9 +3664,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3704,7 +3704,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3810,7 +3810,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3952,7 +3952,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3963,16 +3963,17 @@
   <dimension ref="A1:J268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J256" sqref="J256"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="64.28515625" customWidth="1"/>
-    <col min="9" max="9" width="63.7109375" customWidth="1"/>
+    <col min="3" max="3" width="64.33203125" customWidth="1"/>
+    <col min="9" max="9" width="99.83203125" customWidth="1"/>
+    <col min="10" max="10" width="129.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4001,7 +4002,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>29</v>
       </c>
@@ -4033,7 +4034,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>211</v>
       </c>
@@ -4062,7 +4063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1">
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>149</v>
       </c>
@@ -4091,7 +4092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>165</v>
       </c>
@@ -4123,7 +4124,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>71</v>
       </c>
@@ -4155,7 +4156,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>78</v>
       </c>
@@ -4187,7 +4188,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1">
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>119</v>
       </c>
@@ -4219,7 +4220,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>120</v>
       </c>
@@ -4248,7 +4249,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1">
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>169</v>
       </c>
@@ -4280,7 +4281,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>192</v>
       </c>
@@ -4312,7 +4313,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1">
+    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>194</v>
       </c>
@@ -4341,7 +4342,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="2" customFormat="1">
+    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>44</v>
       </c>
@@ -4373,7 +4374,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1">
+    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>92</v>
       </c>
@@ -4402,7 +4403,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>188</v>
       </c>
@@ -4434,7 +4435,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>238</v>
       </c>
@@ -4466,7 +4467,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="2" customFormat="1">
+    <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>11</v>
       </c>
@@ -4495,7 +4496,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="2" customFormat="1">
+    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>26</v>
       </c>
@@ -4527,7 +4528,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>27</v>
       </c>
@@ -4559,7 +4560,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="2" customFormat="1">
+    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>33</v>
       </c>
@@ -4591,7 +4592,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="2" customFormat="1">
+    <row r="21" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>45</v>
       </c>
@@ -4623,7 +4624,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>54</v>
       </c>
@@ -4655,7 +4656,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="2" customFormat="1">
+    <row r="23" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>69</v>
       </c>
@@ -4687,7 +4688,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="2" customFormat="1">
+    <row r="24" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>102</v>
       </c>
@@ -4716,7 +4717,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>146</v>
       </c>
@@ -4745,7 +4746,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="2" customFormat="1">
+    <row r="26" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>196</v>
       </c>
@@ -4777,7 +4778,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>247</v>
       </c>
@@ -4806,7 +4807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="2" customFormat="1">
+    <row r="28" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>104</v>
       </c>
@@ -4838,7 +4839,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>152</v>
       </c>
@@ -4870,7 +4871,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>77</v>
       </c>
@@ -4902,7 +4903,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>112</v>
       </c>
@@ -4934,7 +4935,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>241</v>
       </c>
@@ -4963,7 +4964,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="2" customFormat="1">
+    <row r="33" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>47</v>
       </c>
@@ -4995,7 +4996,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>123</v>
       </c>
@@ -5027,7 +5028,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>178</v>
       </c>
@@ -5059,7 +5060,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>179</v>
       </c>
@@ -5091,7 +5092,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>181</v>
       </c>
@@ -5123,7 +5124,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>184</v>
       </c>
@@ -5152,7 +5153,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>81</v>
       </c>
@@ -5184,7 +5185,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>204</v>
       </c>
@@ -5216,7 +5217,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>131</v>
       </c>
@@ -5248,7 +5249,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>159</v>
       </c>
@@ -5280,7 +5281,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>176</v>
       </c>
@@ -5312,7 +5313,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>177</v>
       </c>
@@ -5344,7 +5345,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>160</v>
       </c>
@@ -5376,7 +5377,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>175</v>
       </c>
@@ -5408,7 +5409,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>206</v>
       </c>
@@ -5440,7 +5441,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>265</v>
       </c>
@@ -5472,7 +5473,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="2" customFormat="1">
+    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>32</v>
       </c>
@@ -5504,7 +5505,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>76</v>
       </c>
@@ -5533,7 +5534,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>115</v>
       </c>
@@ -5565,7 +5566,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>210</v>
       </c>
@@ -5597,7 +5598,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>212</v>
       </c>
@@ -5629,7 +5630,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>213</v>
       </c>
@@ -5658,7 +5659,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>252</v>
       </c>
@@ -5690,7 +5691,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>253</v>
       </c>
@@ -5722,7 +5723,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="2" customFormat="1">
+    <row r="57" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>13</v>
       </c>
@@ -5751,7 +5752,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>87</v>
       </c>
@@ -5783,7 +5784,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>51</v>
       </c>
@@ -5815,7 +5816,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>56</v>
       </c>
@@ -5847,7 +5848,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5879,7 +5880,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>64</v>
       </c>
@@ -5911,7 +5912,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>197</v>
       </c>
@@ -5943,7 +5944,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>16</v>
       </c>
@@ -5975,7 +5976,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>50</v>
       </c>
@@ -6007,7 +6008,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>21</v>
       </c>
@@ -6039,7 +6040,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>52</v>
       </c>
@@ -6071,7 +6072,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="2" customFormat="1">
+    <row r="68" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>14</v>
       </c>
@@ -6103,7 +6104,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>139</v>
       </c>
@@ -6135,7 +6136,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>148</v>
       </c>
@@ -6167,7 +6168,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>161</v>
       </c>
@@ -6199,7 +6200,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>162</v>
       </c>
@@ -6231,7 +6232,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>173</v>
       </c>
@@ -6260,7 +6261,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>182</v>
       </c>
@@ -6292,7 +6293,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>189</v>
       </c>
@@ -6324,7 +6325,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>200</v>
       </c>
@@ -6353,7 +6354,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>239</v>
       </c>
@@ -6385,7 +6386,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>240</v>
       </c>
@@ -6417,7 +6418,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>150</v>
       </c>
@@ -6449,7 +6450,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>58</v>
       </c>
@@ -6481,7 +6482,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="2" customFormat="1">
+    <row r="81" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>1</v>
       </c>
@@ -6513,7 +6514,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>70</v>
       </c>
@@ -6545,7 +6546,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>138</v>
       </c>
@@ -6577,7 +6578,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>168</v>
       </c>
@@ -6609,7 +6610,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>42</v>
       </c>
@@ -6641,7 +6642,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>126</v>
       </c>
@@ -6670,7 +6671,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>202</v>
       </c>
@@ -6702,7 +6703,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>163</v>
       </c>
@@ -6734,7 +6735,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6763,7 +6764,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>254</v>
       </c>
@@ -6795,7 +6796,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>94</v>
       </c>
@@ -6827,7 +6828,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>246</v>
       </c>
@@ -6859,7 +6860,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>170</v>
       </c>
@@ -6891,7 +6892,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>5</v>
       </c>
@@ -6923,7 +6924,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>95</v>
       </c>
@@ -6955,7 +6956,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>172</v>
       </c>
@@ -6987,7 +6988,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>24</v>
       </c>
@@ -7019,7 +7020,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>73</v>
       </c>
@@ -7051,7 +7052,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>84</v>
       </c>
@@ -7083,7 +7084,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>164</v>
       </c>
@@ -7115,7 +7116,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>180</v>
       </c>
@@ -7147,7 +7148,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>198</v>
       </c>
@@ -7179,7 +7180,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>80</v>
       </c>
@@ -7211,7 +7212,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>242</v>
       </c>
@@ -7243,7 +7244,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>48</v>
       </c>
@@ -7275,7 +7276,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>61</v>
       </c>
@@ -7307,7 +7308,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>74</v>
       </c>
@@ -7339,7 +7340,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>187</v>
       </c>
@@ -7371,7 +7372,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>227</v>
       </c>
@@ -7400,7 +7401,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>228</v>
       </c>
@@ -7432,7 +7433,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>62</v>
       </c>
@@ -7464,7 +7465,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>221</v>
       </c>
@@ -7496,7 +7497,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>141</v>
       </c>
@@ -7528,7 +7529,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>9</v>
       </c>
@@ -7560,7 +7561,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>35</v>
       </c>
@@ -7592,7 +7593,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>193</v>
       </c>
@@ -7624,7 +7625,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="117" spans="1:10" s="2" customFormat="1">
+    <row r="117" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>10</v>
       </c>
@@ -7656,7 +7657,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>39</v>
       </c>
@@ -7688,7 +7689,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>4</v>
       </c>
@@ -7720,7 +7721,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>55</v>
       </c>
@@ -7752,7 +7753,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>86</v>
       </c>
@@ -7784,7 +7785,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>98</v>
       </c>
@@ -7816,7 +7817,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>101</v>
       </c>
@@ -7845,7 +7846,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>113</v>
       </c>
@@ -7877,7 +7878,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>186</v>
       </c>
@@ -7906,7 +7907,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>203</v>
       </c>
@@ -7938,7 +7939,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>236</v>
       </c>
@@ -7967,7 +7968,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>250</v>
       </c>
@@ -7999,7 +8000,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>257</v>
       </c>
@@ -8028,7 +8029,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>231</v>
       </c>
@@ -8060,7 +8061,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="131" spans="1:10" s="2" customFormat="1">
+    <row r="131" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>18</v>
       </c>
@@ -8092,7 +8093,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>111</v>
       </c>
@@ -8124,7 +8125,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>23</v>
       </c>
@@ -8156,7 +8157,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>121</v>
       </c>
@@ -8188,7 +8189,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>151</v>
       </c>
@@ -8220,7 +8221,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>205</v>
       </c>
@@ -8252,7 +8253,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>153</v>
       </c>
@@ -8284,7 +8285,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>130</v>
       </c>
@@ -8316,7 +8317,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>83</v>
       </c>
@@ -8348,7 +8349,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>91</v>
       </c>
@@ -8380,7 +8381,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>233</v>
       </c>
@@ -8412,7 +8413,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>106</v>
       </c>
@@ -8444,7 +8445,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>157</v>
       </c>
@@ -8473,7 +8474,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>214</v>
       </c>
@@ -8505,7 +8506,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>226</v>
       </c>
@@ -8537,7 +8538,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>57</v>
       </c>
@@ -8569,7 +8570,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>127</v>
       </c>
@@ -8601,7 +8602,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>244</v>
       </c>
@@ -8633,7 +8634,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>20</v>
       </c>
@@ -8665,7 +8666,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>100</v>
       </c>
@@ -8697,7 +8698,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>108</v>
       </c>
@@ -8729,7 +8730,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>116</v>
       </c>
@@ -8761,7 +8762,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>224</v>
       </c>
@@ -8793,7 +8794,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>40</v>
       </c>
@@ -8825,7 +8826,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>65</v>
       </c>
@@ -8857,7 +8858,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>89</v>
       </c>
@@ -8886,7 +8887,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>166</v>
       </c>
@@ -8918,7 +8919,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>190</v>
       </c>
@@ -8950,7 +8951,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>8</v>
       </c>
@@ -8982,7 +8983,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>133</v>
       </c>
@@ -9011,7 +9012,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>258</v>
       </c>
@@ -9043,7 +9044,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>125</v>
       </c>
@@ -9075,7 +9076,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>82</v>
       </c>
@@ -9104,7 +9105,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>140</v>
       </c>
@@ -9136,7 +9137,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>142</v>
       </c>
@@ -9168,7 +9169,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>22</v>
       </c>
@@ -9200,7 +9201,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>110</v>
       </c>
@@ -9232,7 +9233,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>199</v>
       </c>
@@ -9264,7 +9265,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>59</v>
       </c>
@@ -9296,7 +9297,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>266</v>
       </c>
@@ -9325,7 +9326,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>68</v>
       </c>
@@ -9357,7 +9358,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>38</v>
       </c>
@@ -9389,7 +9390,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>46</v>
       </c>
@@ -9421,7 +9422,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>107</v>
       </c>
@@ -9453,7 +9454,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>117</v>
       </c>
@@ -9482,7 +9483,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>185</v>
       </c>
@@ -9514,7 +9515,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>245</v>
       </c>
@@ -9546,7 +9547,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>249</v>
       </c>
@@ -9575,7 +9576,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>267</v>
       </c>
@@ -9607,7 +9608,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>137</v>
       </c>
@@ -9639,7 +9640,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>136</v>
       </c>
@@ -9671,7 +9672,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>230</v>
       </c>
@@ -9703,7 +9704,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>234</v>
       </c>
@@ -9735,7 +9736,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>256</v>
       </c>
@@ -9767,7 +9768,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>135</v>
       </c>
@@ -9799,7 +9800,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>17</v>
       </c>
@@ -9831,7 +9832,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>156</v>
       </c>
@@ -9863,7 +9864,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>191</v>
       </c>
@@ -9895,7 +9896,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>217</v>
       </c>
@@ -9924,7 +9925,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>28</v>
       </c>
@@ -9956,7 +9957,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>67</v>
       </c>
@@ -9988,7 +9989,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>6</v>
       </c>
@@ -10020,7 +10021,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>19</v>
       </c>
@@ -10052,7 +10053,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>43</v>
       </c>
@@ -10084,7 +10085,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>97</v>
       </c>
@@ -10116,7 +10117,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>262</v>
       </c>
@@ -10145,7 +10146,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>128</v>
       </c>
@@ -10177,7 +10178,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>118</v>
       </c>
@@ -10209,7 +10210,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>259</v>
       </c>
@@ -10241,7 +10242,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>93</v>
       </c>
@@ -10273,7 +10274,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>145</v>
       </c>
@@ -10305,7 +10306,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>34</v>
       </c>
@@ -10337,7 +10338,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>223</v>
       </c>
@@ -10369,7 +10370,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>143</v>
       </c>
@@ -10401,7 +10402,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>2</v>
       </c>
@@ -10433,7 +10434,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>144</v>
       </c>
@@ -10465,7 +10466,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>183</v>
       </c>
@@ -10497,7 +10498,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>7</v>
       </c>
@@ -10529,7 +10530,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>90</v>
       </c>
@@ -10561,7 +10562,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>147</v>
       </c>
@@ -10593,7 +10594,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>219</v>
       </c>
@@ -10622,7 +10623,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>235</v>
       </c>
@@ -10654,7 +10655,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>243</v>
       </c>
@@ -10686,7 +10687,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>264</v>
       </c>
@@ -10718,7 +10719,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>122</v>
       </c>
@@ -10750,7 +10751,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>75</v>
       </c>
@@ -10782,7 +10783,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>66</v>
       </c>
@@ -10814,7 +10815,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>49</v>
       </c>
@@ -10846,7 +10847,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>260</v>
       </c>
@@ -10878,7 +10879,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>85</v>
       </c>
@@ -10910,7 +10911,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>232</v>
       </c>
@@ -10942,7 +10943,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>129</v>
       </c>
@@ -10974,7 +10975,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>3</v>
       </c>
@@ -11006,7 +11007,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>222</v>
       </c>
@@ -11038,7 +11039,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>132</v>
       </c>
@@ -11070,7 +11071,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>72</v>
       </c>
@@ -11099,7 +11100,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>201</v>
       </c>
@@ -11131,7 +11132,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>167</v>
       </c>
@@ -11163,7 +11164,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>158</v>
       </c>
@@ -11195,7 +11196,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>31</v>
       </c>
@@ -11227,7 +11228,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>15</v>
       </c>
@@ -11259,7 +11260,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>171</v>
       </c>
@@ -11288,7 +11289,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>216</v>
       </c>
@@ -11320,7 +11321,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>237</v>
       </c>
@@ -11352,7 +11353,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>154</v>
       </c>
@@ -11384,7 +11385,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>37</v>
       </c>
@@ -11416,7 +11417,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>255</v>
       </c>
@@ -11448,7 +11449,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>96</v>
       </c>
@@ -11480,7 +11481,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>155</v>
       </c>
@@ -11512,7 +11513,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>229</v>
       </c>
@@ -11544,7 +11545,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>207</v>
       </c>
@@ -11576,7 +11577,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>225</v>
       </c>
@@ -11608,7 +11609,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
         <v>12</v>
       </c>
@@ -11640,7 +11641,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>99</v>
       </c>
@@ -11672,7 +11673,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>209</v>
       </c>
@@ -11704,7 +11705,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>105</v>
       </c>
@@ -11736,7 +11737,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>174</v>
       </c>
@@ -11768,7 +11769,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>195</v>
       </c>
@@ -11800,7 +11801,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>41</v>
       </c>
@@ -11832,7 +11833,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>134</v>
       </c>
@@ -11864,7 +11865,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>109</v>
       </c>
@@ -11896,7 +11897,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>63</v>
       </c>
@@ -11928,7 +11929,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>215</v>
       </c>
@@ -11960,7 +11961,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>124</v>
       </c>
@@ -11992,7 +11993,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>248</v>
       </c>
@@ -12024,7 +12025,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>103</v>
       </c>
@@ -12056,7 +12057,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>218</v>
       </c>
@@ -12088,7 +12089,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>30</v>
       </c>
@@ -12120,7 +12121,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>36</v>
       </c>
@@ -12152,7 +12153,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>25</v>
       </c>
@@ -12184,7 +12185,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>53</v>
       </c>
@@ -12216,7 +12217,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>79</v>
       </c>
@@ -12248,7 +12249,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>114</v>
       </c>
@@ -12280,7 +12281,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>208</v>
       </c>
@@ -12312,7 +12313,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>220</v>
       </c>
@@ -12344,7 +12345,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>261</v>
       </c>
@@ -12376,7 +12377,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>263</v>
       </c>
@@ -12408,7 +12409,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>251</v>
       </c>

</xml_diff>